<commit_message>
added a lot of changes
</commit_message>
<xml_diff>
--- a/Lab Two - Classification/Lab 2 model scores.xlsx
+++ b/Lab Two - Classification/Lab 2 model scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drsco\Documents\GitHub\machine learning mini proj\final mini\MachineLearning1\Lab Two - Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A3745C-6485-47DE-A3B1-98F5A3075722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE27ED96-499D-48C7-9953-080336172DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EC2E58F1-11EA-474E-BCD0-1EB94D66AFE9}"/>
   </bookViews>
@@ -434,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{744C3F71-2007-416E-B96C-CE42DBA83CBB}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,10 +446,10 @@
     <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,43 +466,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.82732147897262198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>0.82732000000000006</v>
+      </c>
+      <c r="D2">
+        <v>0.90854999999999997</v>
+      </c>
+      <c r="E2">
+        <v>0.74912000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.75890000000000002</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.81525000000000003</v>
+      <c r="C3">
+        <v>0.78837000000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.89137</v>
       </c>
       <c r="E3">
-        <v>0.70399999999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.68340999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>0.74406000000000005</v>
+      </c>
+      <c r="D4">
+        <v>0.85857000000000006</v>
+      </c>
+      <c r="E4">
+        <v>0.61834999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -510,7 +525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -518,13 +533,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix errors and acc
</commit_message>
<xml_diff>
--- a/Lab Two - Classification/Lab 2 model scores.xlsx
+++ b/Lab Two - Classification/Lab 2 model scores.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drsco\Documents\GitHub\machine learning mini proj\final mini\MachineLearning1\Lab Two - Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D86B34C-AD32-4B3E-885B-5253C7245929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D52912-738D-47C3-80B6-4670E79F6E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EC2E58F1-11EA-474E-BCD0-1EB94D66AFE9}"/>
+    <workbookView xWindow="960" yWindow="-15210" windowWidth="17280" windowHeight="8970" xr2:uid="{EC2E58F1-11EA-474E-BCD0-1EB94D66AFE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
   <si>
     <t>Model Type</t>
   </si>
@@ -64,12 +65,255 @@
   </si>
   <si>
     <t>Phase of Flight</t>
+  </si>
+  <si>
+    <t>Variable name</t>
+  </si>
+  <si>
+    <t>Continuous or Categorical</t>
+  </si>
+  <si>
+    <t>Explanation of Variable</t>
+  </si>
+  <si>
+    <t>acft_make</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>Name of the manufacturer of the involved aircraft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acft_model   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The full alphanumeric aircraft model code, including any applicable series or derivative identifiers.     </t>
+  </si>
+  <si>
+    <t>cert_max_gr_wt</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>The actual certificated max gross weight for the aircraft involved in the occurrence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acft_category   </t>
+  </si>
+  <si>
+    <t>The category of the involved aircraft, the definition of aircraft category is the same as that used with respect to the certification, ratings, and privileges</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>Indicates the severity of damage to the accident aircraft. For the purposes of this variable, aircraft damage categories are defined in 49 CFR 830.2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">far_part           </t>
+  </si>
+  <si>
+    <t>The applicable regulation part (14 CFR) or authority the aircraft was operating under at the time of the accident.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afm_hrs_last_insp  </t>
+  </si>
+  <si>
+    <t>The total number of operating hours accumulated on the aircraft airframe since the last inspection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_fly           </t>
+  </si>
+  <si>
+    <t>If the accident aircraft was operating under 14 CFR part 91,103,133, or 137, this was the primary purpose of flight.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dprt_state         </t>
+  </si>
+  <si>
+    <t>The state address of the involved aircraft's last departure point prior to the event.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rwy_len            </t>
+  </si>
+  <si>
+    <t>If the involved aircraft was taking off, landing, or on approach to a designated runway, this refers to the actual length available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rwy_width          </t>
+  </si>
+  <si>
+    <t>If the involved aircraft was taking off, landing, or on approach to a designated runway, this refers to the runway width and indicates the units (meters/feet) of measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ev_type            </t>
+  </si>
+  <si>
+    <t>Refers to a regulatory definition of the event severity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ev_city            </t>
+  </si>
+  <si>
+    <t>The city or place location closest to the site of the event.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ev_state           </t>
+  </si>
+  <si>
+    <t>The state in which the event occurred (if in the US).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ev_country         </t>
+  </si>
+  <si>
+    <t>The country in which the event took place.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sky_cond_ceil      </t>
+  </si>
+  <si>
+    <t>The type of cloud coverage that best describes the cloud ceiling at the time of the accident. A ceiling is defined as any cloud layer of greater than 4/8 coverage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sky_cond_nonceil   </t>
+  </si>
+  <si>
+    <t>The cloud condition (non-ceiling) type present at the time of the event. Indicate the cloud condition (non-ceiling) type present at the time of the event. A non-ceiling is defined as any cloud layer of 4/8 or less coverage, including any cloud layer reported as "few," "scattered," or includes classifications of "thin" or "partial."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wx_int_precip      </t>
+  </si>
+  <si>
+    <t>official FAA/NWS METAR weather reporting codes used to report precipitation intensity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phase_flt_spec     </t>
+  </si>
+  <si>
+    <t>information about the phase of flight in which the occurrence took place.</t>
+  </si>
+  <si>
+    <t>Number of injuries that occurred during the event .</t>
+  </si>
+  <si>
+    <t>Continuous /Categorical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acft_make               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acft_model              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cert_max_gr_wt          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acft_category           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">far_part                </t>
+  </si>
+  <si>
+    <t>afm_hrs_last_insp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_fly                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dprt_state              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rwy_len                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rwy_width               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ev_type                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ev_state                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ev_country              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inj_f_grnd              </t>
+  </si>
+  <si>
+    <t>Number of persons on the ground who were involved in the event who received fatal injuries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inj_m_grnd              </t>
+  </si>
+  <si>
+    <t>Number of persons on the ground who were involved in the event who received no injuries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inj_s_grnd              </t>
+  </si>
+  <si>
+    <t>Number of persons on the ground who were involved in the event who received serious injuries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total_Fatal_Injuries    </t>
+  </si>
+  <si>
+    <t>Number of total fatal injuries that occurred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total_Minor_Injuries    </t>
+  </si>
+  <si>
+    <t>Number of total Minor injuries that occurred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total_Uninjured         </t>
+  </si>
+  <si>
+    <t>Number of total uninjured passengers and crew.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total_Serious_Injuries  </t>
+  </si>
+  <si>
+    <t>Number of total Serious  injuries that occurred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total_Injuries_Flight   </t>
+  </si>
+  <si>
+    <t>Number of total injuries that occurred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sky_cond_ceil           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sky_cond_nonceil        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">wx_int_precip           </t>
+  </si>
+  <si>
+    <t>Official FAA/NWS METAR weather reporting codes used to report precipitation intensity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phase_flt_spec          </t>
+  </si>
+  <si>
+    <t>Information about the phase of flight in which the occurrence took place.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,7 +346,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,15 +354,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,13 +701,13 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" customWidth="1"/>
@@ -524,6 +788,15 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="5">
+        <v>0.55607751027598296</v>
+      </c>
+      <c r="D5">
+        <v>0.407861567298063</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.20934089362976399</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -532,6 +805,15 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6" s="5">
+        <v>0.55020551967116804</v>
+      </c>
+      <c r="D6">
+        <v>0.445079638417199</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.27462677200291702</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -540,6 +822,15 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" s="5">
+        <v>0.25954198473282403</v>
+      </c>
+      <c r="D7">
+        <v>0.18582458429920201</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.33276945270316899</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E11" s="2"/>
@@ -551,6 +842,554 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46645D25-D2E8-4AA6-AC9E-CE3538B8F89B}">
+  <dimension ref="A1:C50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:C50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>